<commit_message>
Modificação da biblioteca, acerto feedback de cadastro de projeto, insere grid com dados na importação AIF
</commit_message>
<xml_diff>
--- a/Files/AIF Mexico - Data Base V2.xlsx
+++ b/Files/AIF Mexico - Data Base V2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LeiteI\Desktop\Sedog Mexico - Latin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{122E6A31-F149-42F7-99B0-ED21E776412B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49950139-BC82-43E2-81A4-8D66849D78EF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{39A6323D-5972-49A1-BF42-F6B03FCF2C95}"/>
   </bookViews>
@@ -6285,7 +6285,7 @@
   <dimension ref="B2:K54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>